<commit_message>
completed uni-variate release 2
</commit_message>
<xml_diff>
--- a/Data/column complete status.xlsx
+++ b/Data/column complete status.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\LendingClubEDA\test_sameer\LendingClubEDA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED79E80-0F3B-4B39-9753-220C6CD956F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF99F5E-8616-4C47-A029-33F63A52B48E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="271">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -773,6 +774,69 @@
   </si>
   <si>
     <t>The first 3 numbers of the zip code provided by the borrower in the loan application.</t>
+  </si>
+  <si>
+    <t>column1</t>
+  </si>
+  <si>
+    <t>column2</t>
+  </si>
+  <si>
+    <t>verificaton_status</t>
+  </si>
+  <si>
+    <t>last_paymnt_d - issue_d / term</t>
+  </si>
+  <si>
+    <t>months_left</t>
+  </si>
+  <si>
+    <t>late_fee_perc</t>
+  </si>
+  <si>
+    <t>out_prncp_perc</t>
+  </si>
+  <si>
+    <t>(out_prncp/loan_amnt)*100</t>
+  </si>
+  <si>
+    <t>(total_rec_late_fee/loan_amnt)*100</t>
+  </si>
+  <si>
+    <t>revol_bal/installement</t>
+  </si>
+  <si>
+    <t>How many times his monthly EMI is his revol bal</t>
+  </si>
+  <si>
+    <t>credit_longetivity</t>
+  </si>
+  <si>
+    <t>Number of months he has stayed with the bank since he got the credit line</t>
+  </si>
+  <si>
+    <t>last_payment_d-earliest_cr_line</t>
+  </si>
+  <si>
+    <t>verified_defaulter</t>
+  </si>
+  <si>
+    <t>if defaulter is verified or not</t>
+  </si>
+  <si>
+    <t>total_payment_perc</t>
+  </si>
+  <si>
+    <t>total_payment/loan_amnt</t>
+  </si>
+  <si>
+    <t>proportion of interst reveived</t>
+  </si>
+  <si>
+    <t>will give prop of interest received</t>
+  </si>
+  <si>
+    <t>receieved_interest * term/((last_paymnt_d - issue_d ) x int_rate x prncp )</t>
   </si>
 </sst>
 </file>
@@ -802,7 +866,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -824,6 +888,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -878,6 +948,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,170 +1287,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E17" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E18" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E19" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E22" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>255</v>
+      </c>
+      <c r="E30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>259</v>
+      </c>
+      <c r="F32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>261</v>
+      </c>
+      <c r="E33" t="s">
+        <v>263</v>
+      </c>
+      <c r="F33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>264</v>
+      </c>
+      <c r="F34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>266</v>
+      </c>
+      <c r="E35" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>268</v>
+      </c>
+      <c r="E36" t="s">
+        <v>270</v>
+      </c>
+      <c r="F36" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1392,11 +1610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="81.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -2341,4 +2562,18 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A5F720-3DEB-492A-AA66-EA17BAE73C7D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="C9:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added 7 bivariate analysis on income bucket and purpose
</commit_message>
<xml_diff>
--- a/Data/column complete status.xlsx
+++ b/Data/column complete status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\LendingClubEDA\test_sameer\LendingClubEDA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A02C8D2-140C-46CE-BF7E-D1004CD27AE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEF319B-16C1-4FB8-A01B-A049C86D7E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="278">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -828,6 +828,36 @@
   </si>
   <si>
     <t>total_payment/loan_amnt</t>
+  </si>
+  <si>
+    <t>revol_bal_mult</t>
+  </si>
+  <si>
+    <t>total_prncp_paid_perc</t>
+  </si>
+  <si>
+    <t>tenure_paid</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>subgrade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
+  </si>
+  <si>
+    <t>loan_bucket</t>
+  </si>
+  <si>
+    <t>loan_bcuket</t>
+  </si>
+  <si>
+    <t>income_bucket</t>
+  </si>
+  <si>
+    <t>loam_amnt_bucket</t>
   </si>
 </sst>
 </file>
@@ -857,7 +887,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -894,6 +924,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -922,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -948,6 +984,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1286,290 +1323,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
       <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="I6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>274</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>275</v>
+      </c>
+      <c r="J16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I20" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I21" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="B29" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="E29" t="s">
+      <c r="C29" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="B30" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E30" t="s">
+      <c r="C30" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="14" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="E31" t="s">
+      <c r="C31" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="13" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
+      <c r="C32" t="s">
         <v>259</v>
       </c>
-      <c r="F32" t="s">
+      <c r="D32" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" t="s">
+        <v>263</v>
+      </c>
       <c r="D33" t="s">
-        <v>261</v>
-      </c>
-      <c r="E33" t="s">
-        <v>263</v>
-      </c>
-      <c r="F33" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="14" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="F34" t="s">
+      <c r="D34" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="13" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E35" t="s">
+      <c r="C35" t="s">
         <v>267</v>
       </c>
     </row>
@@ -1761,7 +1961,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>71</v>
       </c>
@@ -1785,7 +1985,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>77</v>
       </c>
@@ -1793,7 +1993,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>79</v>
       </c>
@@ -1801,7 +2001,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>18</v>
       </c>
@@ -1809,7 +2009,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>21</v>
       </c>
@@ -1817,7 +2017,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>83</v>
       </c>
@@ -1857,7 +2057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -1865,7 +2065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>95</v>
       </c>
@@ -1873,7 +2073,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>97</v>
       </c>
@@ -1881,7 +2081,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>99</v>
       </c>
@@ -1889,7 +2089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>101</v>
       </c>
@@ -1913,7 +2113,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>107</v>
       </c>
@@ -1921,7 +2121,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>109</v>
       </c>
@@ -1929,7 +2129,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>17</v>
       </c>
@@ -1937,7 +2137,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>24</v>
       </c>
@@ -1953,7 +2153,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>115</v>
       </c>
@@ -2001,7 +2201,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>127</v>
       </c>
@@ -2017,7 +2217,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>131</v>
       </c>
@@ -2065,7 +2265,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>143</v>
       </c>
@@ -2185,7 +2385,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>173</v>
       </c>
@@ -2241,7 +2441,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>187</v>
       </c>
@@ -2249,7 +2449,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>189</v>
       </c>
@@ -2273,7 +2473,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>195</v>
       </c>
@@ -2281,7 +2481,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>1</v>
       </c>
@@ -2297,7 +2497,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>25</v>
       </c>
@@ -2305,7 +2505,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>200</v>
       </c>
@@ -2313,7 +2513,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>202</v>
       </c>
@@ -2321,7 +2521,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>2</v>
       </c>
@@ -2329,7 +2529,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
@@ -2337,7 +2537,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>19</v>
       </c>
@@ -2353,7 +2553,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>209</v>
       </c>
@@ -2361,7 +2561,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>211</v>
       </c>
@@ -2393,7 +2593,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>4</v>
       </c>
@@ -2441,7 +2641,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>230</v>
       </c>
@@ -2449,7 +2649,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>232</v>
       </c>
@@ -2457,7 +2657,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>234</v>
       </c>
@@ -2465,7 +2665,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>236</v>
       </c>

</xml_diff>